<commit_message>
UC-1 og navngivning, OC template og UC1-OC
</commit_message>
<xml_diff>
--- a/UPDokument/NavngivningForm.xlsx
+++ b/UPDokument/NavngivningForm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
   <si>
     <t>Navngivning</t>
   </si>
@@ -201,28 +201,28 @@
     <t>FS-UC1-seHistorik-AD</t>
   </si>
   <si>
-    <t>FS-A.# : navn</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
     <t>name for each oc</t>
   </si>
   <si>
-    <t>FS-A : navn</t>
-  </si>
-  <si>
     <t>UC number goes to A</t>
   </si>
   <si>
-    <t>FS-1 : seHistorik</t>
-  </si>
-  <si>
-    <t>FS-1.1 : seHistorik</t>
-  </si>
-  <si>
     <t>FS-1.2 : angivOplysninger</t>
+  </si>
+  <si>
+    <t>FS-OC1.1 : seHistorik</t>
+  </si>
+  <si>
+    <t>remember to check Anders ppt (OOA-6)</t>
+  </si>
+  <si>
+    <t>FS-UC1 : seHistorik</t>
+  </si>
+  <si>
+    <t>FS-OC#.# : navn</t>
   </si>
 </sst>
 </file>
@@ -561,7 +561,7 @@
   <dimension ref="A2:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,7 +571,7 @@
     <col min="3" max="3" width="23" style="1" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
@@ -703,16 +703,16 @@
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>22</v>
@@ -720,13 +720,13 @@
     </row>
     <row r="20" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>20</v>
@@ -734,10 +734,13 @@
       <c r="E20" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="F20" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
DCD fixed, need to ask Anders. Report
</commit_message>
<xml_diff>
--- a/UPDokument/NavngivningForm.xlsx
+++ b/UPDokument/NavngivningForm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
   <si>
     <t>Navngivning</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>title in each visio diagram</t>
+  </si>
+  <si>
+    <t>OC#.#-DCD: navn</t>
   </si>
 </sst>
 </file>
@@ -561,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F33"/>
+  <dimension ref="A2:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -845,6 +848,11 @@
       </c>
       <c r="E33" s="3" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>